<commit_message>
Cambios en algunos archivos
</commit_message>
<xml_diff>
--- a/Materiales Del Curso Originales/dt_ptl_controlAsignaciones.xlsx
+++ b/Materiales Del Curso Originales/dt_ptl_controlAsignaciones.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="71" documentId="9BEF71734ADC2BAB9176336787A8638BDC4A3CE7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{07AF016F-8F2B-412F-833E-0293463D6785}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MetodosFormalesSoftware\Materiales Del Curso Originales\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4E594949-CAD1-4D0F-80F4-F4CFF4A573BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SEMANA 1'!$A$7:$N$7</definedName>
   </definedNames>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -28,12 +33,6 @@
     <t>Universidad Piloto de Colombia</t>
   </si>
   <si>
-    <t xml:space="preserve">PROYECTO:  </t>
-  </si>
-  <si>
-    <t>Grupo:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ciclo: </t>
   </si>
   <si>
@@ -215,6 +214,12 @@
   </si>
   <si>
     <t>Elaborar el Informe semanal</t>
+  </si>
+  <si>
+    <t>Grupo: OASIS</t>
+  </si>
+  <si>
+    <t>PROYECTO:  Propiedades para vacacionar</t>
   </si>
 </sst>
 </file>
@@ -226,7 +231,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -545,6 +550,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,12 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -994,11 +999,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -1010,164 +1015,166 @@
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32.25" customHeight="1">
-      <c r="A1" s="28"/>
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30"/>
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
-    </row>
-    <row r="2" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35"/>
-    </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="35"/>
+    </row>
+    <row r="2" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="43"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="39"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="40" t="s">
+      <c r="N4" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="29"/>
+    </row>
+    <row r="7" spans="1:14" s="20" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="41"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="37"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="23"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="27"/>
-    </row>
-    <row r="7" spans="1:14" s="20" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="C7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="D7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="E7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="G7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="H7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="I7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="K7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="L7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="M7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="N7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="22" t="s">
+    </row>
+    <row r="8" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="D8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="G8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42" t="s">
+      <c r="H8" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>25</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="11"/>
@@ -1176,28 +1183,28 @@
       <c r="M8" s="8"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="9" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="G9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42" t="s">
+      <c r="H9" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>25</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="11"/>
@@ -1206,28 +1213,28 @@
       <c r="M9" s="8"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="10" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="G10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42" t="s">
+      <c r="H10" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>25</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="11"/>
@@ -1236,28 +1243,28 @@
       <c r="M10" s="8"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="42" t="s">
+      <c r="G11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42" t="s">
+      <c r="H11" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>25</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="11"/>
@@ -1266,28 +1273,28 @@
       <c r="M11" s="8"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="12" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="G12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42" t="s">
+      <c r="H12" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>25</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="11"/>
@@ -1296,28 +1303,28 @@
       <c r="M12" s="8"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="13" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>31</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="11"/>
@@ -1326,28 +1333,28 @@
       <c r="M13" s="8"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="14" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="42" t="s">
+      <c r="H14" s="26" t="s">
         <v>33</v>
-      </c>
-      <c r="G14" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>35</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="11"/>
@@ -1356,28 +1363,28 @@
       <c r="M14" s="8"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" s="6" customFormat="1" ht="36.75" customHeight="1">
+    <row r="15" spans="1:14" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="G15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>40</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="11"/>
@@ -1386,28 +1393,28 @@
       <c r="M15" s="8"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="16" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="43" t="s">
-        <v>43</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="11"/>
@@ -1416,9 +1423,9 @@
       <c r="M16" s="8"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="17" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1434,9 +1441,9 @@
       <c r="M17" s="8"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="18" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1452,9 +1459,9 @@
       <c r="M18" s="8"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="19" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1470,9 +1477,9 @@
       <c r="M19" s="8"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1488,9 +1495,9 @@
       <c r="M20" s="16"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="21" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1506,9 +1513,9 @@
       <c r="M21" s="8"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="22" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1524,9 +1531,9 @@
       <c r="M22" s="8"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="23" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1542,9 +1549,9 @@
       <c r="M23" s="8"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="24" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1560,9 +1567,9 @@
       <c r="M24" s="8"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="25" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1578,9 +1585,9 @@
       <c r="M25" s="8"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="26" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1596,9 +1603,9 @@
       <c r="M26" s="8"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="27" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1614,9 +1621,9 @@
       <c r="M27" s="8"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="28" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1632,9 +1639,9 @@
       <c r="M28" s="8"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="29" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1650,9 +1657,9 @@
       <c r="M29" s="8"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="30" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1668,9 +1675,9 @@
       <c r="M30" s="8"/>
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="31" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1686,9 +1693,9 @@
       <c r="M31" s="8"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="32" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1704,9 +1711,9 @@
       <c r="M32" s="8"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="33" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1722,9 +1729,9 @@
       <c r="M33" s="8"/>
       <c r="N33" s="7"/>
     </row>
-    <row r="34" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="34" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -1740,9 +1747,9 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="35" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -1758,9 +1765,9 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1">
+    <row r="36" spans="1:14" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -1776,9 +1783,9 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="37" spans="1:14" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -1794,22 +1801,22 @@
       <c r="M37" s="8"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N43" s="5"/>
     </row>
   </sheetData>
@@ -1834,9 +1841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89075FB3-E8EE-429F-AB63-6E38727FABC0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{5F651639-E4D3-5662-A7AE-48FF4BA4D9D9}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1846,9 +1853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591A9275-8853-4DD0-990D-C389F4C65382}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{5D3C7988-DF0D-529A-8A07-078F9E5FDBE5}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>